<commit_message>
changes to test cases outline
</commit_message>
<xml_diff>
--- a/p5/TestCases.xlsx
+++ b/p5/TestCases.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\d_gra\Documents\Queen's\Fourth Year Eng\CISC 327\Assignment Repo\p5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikem\Documents\Queen's\Senior\327\a1\327-Part-1\p5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5E8998-38FA-4577-BF18-F5E342840BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8975F059-D603-4058-A77C-6E2FED217393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B10D695A-5E97-46FB-B90E-09D4C431AB42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B10D695A-5E97-46FB-B90E-09D4C431AB42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Withdraw" sheetId="1" r:id="rId1"/>
+    <sheet name="Create" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
   <si>
     <t>Decision</t>
   </si>
@@ -177,12 +178,129 @@
   <si>
     <t>Statement</t>
   </si>
+  <si>
+    <t>White Box Test #1: Withdraw</t>
+  </si>
+  <si>
+    <t>1. Code Section Being Tested:</t>
+  </si>
+  <si>
+    <t>2. Test Case Analysis</t>
+  </si>
+  <si>
+    <t>For the withdraw method, the team has decided to use decision coverage. Since there are two if statements (marked above</t>
+  </si>
+  <si>
+    <t xml:space="preserve">with 1 and 2), there will be 4 possible test cases. (True-True, True-False, False-True, False-False). These cases will cover </t>
+  </si>
+  <si>
+    <t>all possible decisions in this method.</t>
+  </si>
+  <si>
+    <t>3. Test Inputs</t>
+  </si>
+  <si>
+    <t>The following inputs were used as test inputs for the decision testing.</t>
+  </si>
+  <si>
+    <t>4. Test Results</t>
+  </si>
+  <si>
+    <t>The following test results were observed from the testing inputs above.</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>Success (Y/N)</t>
+  </si>
+  <si>
+    <t>Decision 1 (accountActive == 1)</t>
+  </si>
+  <si>
+    <t>Decision 2 (newBal &gt; 0)</t>
+  </si>
+  <si>
+    <t>TSF statement</t>
+  </si>
+  <si>
+    <t>WDR 1234567 1000 0000000 ***</t>
+  </si>
+  <si>
+    <t>WDR 1234567 999999999 0000000 ***</t>
+  </si>
+  <si>
+    <t>WDR 2468246 1000 0000000 ***</t>
+  </si>
+  <si>
+    <t>WDR 2468246 999999999 0000000 ***</t>
+  </si>
+  <si>
+    <t>*******THE ORIGINAL TESTING ONE WE HAD IS ABOVE, I THINK THE ONE BELOW FITS THEIR REQUIREMENTS BETTER*************</t>
+  </si>
+  <si>
+    <t>Successful transaction, 1000 withdrawn from account 1234567.</t>
+  </si>
+  <si>
+    <t>Unsuccessful transaction, "Failed Constraint: Account was deleted"</t>
+  </si>
+  <si>
+    <t>Unsuccessful transaction, "Failed Constraint: insufficient funds"</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>White Box Test #2: Create</t>
+  </si>
+  <si>
+    <t>For the create method, the team has decided to use statement coverage. Since there is only one statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plus the if statement, only two mutants need to be created as test inputs. </t>
+  </si>
+  <si>
+    <t>*ABOVE:previous, BELOW: new(</t>
+  </si>
+  <si>
+    <t>No change to accountsHash or VAF/MAF</t>
+  </si>
+  <si>
+    <t>T1a</t>
+  </si>
+  <si>
+    <t>T1b</t>
+  </si>
+  <si>
+    <t>Valid account created and added to VAF/MAF</t>
+  </si>
+  <si>
+    <t>Invalid account created and added to VAF/MAF</t>
+  </si>
+  <si>
+    <t>Valid (Y/N)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>NEW 1234567 000 0000000 Bob #where accNum 1234567 exists)</t>
+  </si>
+  <si>
+    <t>NEW 1234321 000 0000000 Bob #where accNum 1234321 doesn't exist)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -200,6 +318,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -276,77 +402,10 @@
       <right style="thin">
         <color theme="2"/>
       </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color theme="2"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2"/>
-      </left>
-      <right style="thin">
-        <color theme="2"/>
-      </right>
-      <top style="thin">
-        <color theme="2"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -365,21 +424,17 @@
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color theme="2"/>
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -387,22 +442,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,58 +472,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>144118</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2210237</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>102428</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ECB9F41-E498-4C8D-B2EC-7242DD561B27}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="3192118"/>
-          <a:ext cx="6235585" cy="3387310"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>57966</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>6259</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52643</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>594976</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>116477</xdr:rowOff>
+      <xdr:colOff>397863</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>162860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -493,7 +495,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -507,8 +509,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="57966" y="1181916"/>
-          <a:ext cx="6809287" cy="2069647"/>
+          <a:off x="0" y="609234"/>
+          <a:ext cx="6977567" cy="1965522"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -527,25 +529,30 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>132049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1652547</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>410487</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>63469</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A15CF80-E791-4A52-B2D7-08DBBDEBB8C4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69410491-4274-40A9-A90D-8C53D7591FB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -554,7 +561,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -568,8 +575,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="11852414" y="703549"/>
-          <a:ext cx="4211872" cy="693420"/>
+          <a:off x="12123421" y="680689"/>
+          <a:ext cx="4289066" cy="662940"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -584,50 +591,6 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>604631</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>176888</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>228026</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>76145</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3192685-2530-4CC4-B9D8-3CC1C3F55B48}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11844131" y="1510388"/>
-          <a:ext cx="6796134" cy="4280757"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -932,252 +895,580 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F90E1C3-F234-41B2-AE27-09B503EEFE88}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" customWidth="1"/>
-    <col min="13" max="13" width="50.85546875" customWidth="1"/>
-    <col min="15" max="15" width="77.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" customWidth="1"/>
+    <col min="7" max="7" width="33.44140625" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" customWidth="1"/>
+    <col min="13" max="13" width="50.88671875" customWidth="1"/>
+    <col min="15" max="15" width="77.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
-        <v>100</v>
-      </c>
-      <c r="D2" s="2">
-        <v>100</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1234568</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>100</v>
-      </c>
-      <c r="D3" s="2">
-        <v>100</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="2">
-        <v>100</v>
-      </c>
-      <c r="J3" s="3">
-        <v>2</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1234560</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>100</v>
-      </c>
-      <c r="D4" s="2">
-        <v>100</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>100</v>
-      </c>
-      <c r="E5" s="2">
-        <v>-100</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="17"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="16"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="18"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="12"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="11"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>100</v>
+      </c>
+      <c r="D24" s="2">
+        <v>100</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>100</v>
+      </c>
+      <c r="D25" s="2">
+        <v>100</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>100</v>
+      </c>
+      <c r="D26" s="2">
+        <v>100</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2">
+        <v>100</v>
+      </c>
+      <c r="E27" s="2">
+        <v>-100</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="7"/>
       <c r="E28" s="6"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="4"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD60528A-8FE5-4AEF-A540-8FF1EAF5386A}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="42.21875" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="60.21875" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" customWidth="1"/>
+    <col min="6" max="6" width="72.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1234568</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1234560</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>